<commit_message>
Updates for tertiary analyses
</commit_message>
<xml_diff>
--- a/_docs/literature/references.xlsx
+++ b/_docs/literature/references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drewc\neville\Health-Risk-and-Equity\_docs\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B6ADC2-FE68-4B8E-AB35-F72D66416801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4681CB-9FD7-4293-A5D3-A2D6E660FB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{19D679A9-060C-40A9-9FC2-E92FAADFCEF1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="235">
   <si>
     <t>Title</t>
   </si>
@@ -726,6 +726,21 @@
   </si>
   <si>
     <t>A Theory of Justice - John Rawls - Google Books</t>
+  </si>
+  <si>
+    <t>Kitigawa, Evelyn M</t>
+  </si>
+  <si>
+    <t>Components of a Difference Between Two Rates</t>
+  </si>
+  <si>
+    <t>Journal of the American Statistical Association</t>
+  </si>
+  <si>
+    <t>10.2307/2281213</t>
+  </si>
+  <si>
+    <t>W HEN comparing the incidence of some phenomenon in two or more w groups, social researchers place much emphasis on the need for holding constant those related factors that would tend to distort the comparison. For example, before comparing the death rates for the residents of two areas, demographers frequently control the factors of differences between the areas in age, sex and race composition. A tech- nique commonly used to accomplish this is "standardization" of the rates for the two areas by relating them both to a standard population with specified age-sex-race composition. By applying the schedule of age-sex-race specific death rates for each of the groups to the age-sex- race composition of the standard population, then noting the total death rate that results, it is possible to compare the death rates for the areas with reasonable confidence that differences in age, sex and race composition do not explain the differences between the rates for the areas that still remain after they have been standardized. Controlling the effect of related factors by this method is termed direct standard- ization. 1</t>
   </si>
 </sst>
 </file>
@@ -992,7 +1007,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1061,6 +1076,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1376,10 +1392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D8EC48-C9E1-4E22-9047-0DD447A5953A}">
-  <dimension ref="B1:J51"/>
+  <dimension ref="B1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2606,97 +2622,120 @@
         <v>154</v>
       </c>
     </row>
-    <row r="48" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>85</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="8" t="s">
-        <v>86</v>
+        <v>231</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>87</v>
+        <v>232</v>
       </c>
       <c r="H48" s="14">
-        <v>1978</v>
-      </c>
-      <c r="I48" s="17" t="s">
-        <v>88</v>
+        <v>1955</v>
+      </c>
+      <c r="I48" s="36" t="s">
+        <v>233</v>
       </c>
       <c r="J48" s="20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="7" t="s">
-        <v>223</v>
+        <v>84</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>227</v>
+        <v>85</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
       <c r="F49" s="8" t="s">
-        <v>226</v>
+        <v>86</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>194</v>
+        <v>87</v>
       </c>
       <c r="H49" s="14">
-        <v>1974</v>
+        <v>1978</v>
       </c>
       <c r="I49" s="17" t="s">
-        <v>224</v>
+        <v>88</v>
       </c>
       <c r="J49" s="20" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="C50" s="8"/>
+        <v>223</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>227</v>
+      </c>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="H50" s="14">
+        <v>1974</v>
+      </c>
+      <c r="I50" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="J50" s="20" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="G50" s="8" t="s">
+      <c r="G51" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="H50" s="14">
+      <c r="H51" s="14">
         <v>1985</v>
       </c>
-      <c r="I50" s="17" t="s">
+      <c r="I51" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="J50" s="20" t="s">
+      <c r="J51" s="20" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="51" spans="2:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="9" t="s">
+    <row r="52" spans="2:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10" t="s">
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="G51" s="10"/>
-      <c r="H51" s="15">
+      <c r="G52" s="10"/>
+      <c r="H52" s="15">
         <v>1971</v>
       </c>
-      <c r="I51" s="24" t="s">
+      <c r="I52" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="J51" s="22"/>
+      <c r="J52" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2715,7 +2754,7 @@
     <hyperlink ref="I36" r:id="rId13" xr:uid="{F8B71C5E-23B5-461F-A049-EE50E7EFF25C}"/>
     <hyperlink ref="I15" r:id="rId14" xr:uid="{2B48EEBA-2358-4372-B7F0-96CD877BE9F5}"/>
     <hyperlink ref="I9" r:id="rId15" xr:uid="{866D072E-E466-41C6-AD18-6C84D6CDDA6B}"/>
-    <hyperlink ref="I48" r:id="rId16" xr:uid="{970EF78B-408F-4C98-B0D8-88A63CF6FACC}"/>
+    <hyperlink ref="I49" r:id="rId16" xr:uid="{970EF78B-408F-4C98-B0D8-88A63CF6FACC}"/>
     <hyperlink ref="I42" r:id="rId17" xr:uid="{ACB90C54-DD38-44AD-BCC3-534B32190ED1}"/>
     <hyperlink ref="I43" r:id="rId18" xr:uid="{0FA0F87A-954B-4EE3-AF4B-461F05DAA482}"/>
     <hyperlink ref="I44" r:id="rId19" xr:uid="{404169E8-B43B-4E92-919E-526499D71C36}"/>
@@ -2734,10 +2773,11 @@
     <hyperlink ref="I14" r:id="rId32" xr:uid="{364EE8A0-510C-4DD4-B588-97BC64AF5D84}"/>
     <hyperlink ref="I46" r:id="rId33" xr:uid="{5E202092-DCE6-4C0C-A416-C0003D4CDE2C}"/>
     <hyperlink ref="I40" r:id="rId34" xr:uid="{2D11A1FA-5EA8-4BD5-8685-A2595E224191}"/>
-    <hyperlink ref="I50" r:id="rId35" xr:uid="{93BA408A-E308-4AA3-AFF9-D1875E03F4D3}"/>
-    <hyperlink ref="I49" r:id="rId36" xr:uid="{69D1E48E-EDA5-42F5-BD96-ACFA9F0207F0}"/>
+    <hyperlink ref="I51" r:id="rId35" xr:uid="{93BA408A-E308-4AA3-AFF9-D1875E03F4D3}"/>
+    <hyperlink ref="I50" r:id="rId36" xr:uid="{69D1E48E-EDA5-42F5-BD96-ACFA9F0207F0}"/>
+    <hyperlink ref="I48" r:id="rId37" xr:uid="{A32793BB-47E7-42D8-9B27-3D2EA90D7926}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId37"/>
+  <pageSetup orientation="portrait" r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>